<commit_message>
Changes as per request
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/Seller_Test_Data.xlsx
+++ b/MarsFramework/ExcelData/Seller_Test_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pinky Sindhu\Desktop\Industry Connect\Industry Connect\Internship\Task 2\marsframework-master\MarsFramework\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F85F5333-7AB3-41E9-996E-EEF269369784}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1EE9FFA-6108-4B94-8128-3B7386397C7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" activeTab="1" xr2:uid="{47384E78-1A99-4AD6-B104-C46CFD79473E}"/>
   </bookViews>
@@ -134,16 +134,16 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>04-04-2020</t>
-  </si>
-  <si>
-    <t>20-05-2020</t>
-  </si>
-  <si>
     <t>6:00:00 PM</t>
   </si>
   <si>
     <t>8:00:00 PM</t>
+  </si>
+  <si>
+    <t>14/04/2021</t>
+  </si>
+  <si>
+    <t>20/05/2021</t>
   </si>
 </sst>
 </file>
@@ -571,7 +571,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -662,19 +662,19 @@
         <v>27</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>28</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>18</v>

</xml_diff>